<commit_message>
fixed TARGET value log bug
</commit_message>
<xml_diff>
--- a/bank_nifty_stats_report.xlsx
+++ b/bank_nifty_stats_report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3134"/>
+  <dimension ref="A1:H3143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -81924,6 +81924,240 @@
         <v>38232.17459443517</v>
       </c>
     </row>
+    <row r="3135">
+      <c r="A3135" s="1" t="n">
+        <v>3133</v>
+      </c>
+      <c r="B3135" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3135" t="n">
+        <v>38252.5</v>
+      </c>
+      <c r="D3135" t="n">
+        <v>38275.5</v>
+      </c>
+      <c r="E3135" t="n">
+        <v>38202.7</v>
+      </c>
+      <c r="F3135" t="n">
+        <v>38239.5</v>
+      </c>
+      <c r="G3135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3135" t="n">
+        <v>38234.61639629012</v>
+      </c>
+    </row>
+    <row r="3136">
+      <c r="A3136" s="1" t="n">
+        <v>3134</v>
+      </c>
+      <c r="B3136" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3136" t="n">
+        <v>38239.05</v>
+      </c>
+      <c r="D3136" t="n">
+        <v>38245.65</v>
+      </c>
+      <c r="E3136" t="n">
+        <v>38212.45</v>
+      </c>
+      <c r="F3136" t="n">
+        <v>38230.95</v>
+      </c>
+      <c r="G3136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3136" t="n">
+        <v>38233.39426419341</v>
+      </c>
+    </row>
+    <row r="3137">
+      <c r="A3137" s="1" t="n">
+        <v>3135</v>
+      </c>
+      <c r="B3137" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3137" t="n">
+        <v>38232.95</v>
+      </c>
+      <c r="D3137" t="n">
+        <v>38240.75</v>
+      </c>
+      <c r="E3137" t="n">
+        <v>38220.25</v>
+      </c>
+      <c r="F3137" t="n">
+        <v>38238.65</v>
+      </c>
+      <c r="G3137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3137" t="n">
+        <v>38235.14617612894</v>
+      </c>
+    </row>
+    <row r="3138">
+      <c r="A3138" s="1" t="n">
+        <v>3136</v>
+      </c>
+      <c r="B3138" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3138" t="n">
+        <v>38238.35</v>
+      </c>
+      <c r="D3138" t="n">
+        <v>38242.7</v>
+      </c>
+      <c r="E3138" t="n">
+        <v>38211.65</v>
+      </c>
+      <c r="F3138" t="n">
+        <v>38226.4</v>
+      </c>
+      <c r="G3138" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3138" t="n">
+        <v>38232.23078408596</v>
+      </c>
+    </row>
+    <row r="3139">
+      <c r="A3139" s="1" t="n">
+        <v>3137</v>
+      </c>
+      <c r="B3139" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3139" t="n">
+        <v>38230.3</v>
+      </c>
+      <c r="D3139" t="n">
+        <v>38238.25</v>
+      </c>
+      <c r="E3139" t="n">
+        <v>38202.3</v>
+      </c>
+      <c r="F3139" t="n">
+        <v>38227.45</v>
+      </c>
+      <c r="G3139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3139" t="n">
+        <v>38230.63718939065</v>
+      </c>
+    </row>
+    <row r="3140">
+      <c r="A3140" s="1" t="n">
+        <v>3138</v>
+      </c>
+      <c r="B3140" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3140" t="n">
+        <v>38229.15</v>
+      </c>
+      <c r="D3140" t="n">
+        <v>38243.45</v>
+      </c>
+      <c r="E3140" t="n">
+        <v>38219.7</v>
+      </c>
+      <c r="F3140" t="n">
+        <v>38231.1</v>
+      </c>
+      <c r="G3140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3140" t="n">
+        <v>38230.79145959377</v>
+      </c>
+    </row>
+    <row r="3141">
+      <c r="A3141" s="1" t="n">
+        <v>3139</v>
+      </c>
+      <c r="B3141" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3141" t="n">
+        <v>38229.55</v>
+      </c>
+      <c r="D3141" t="n">
+        <v>38261.25</v>
+      </c>
+      <c r="E3141" t="n">
+        <v>38216.8</v>
+      </c>
+      <c r="F3141" t="n">
+        <v>38233.45</v>
+      </c>
+      <c r="G3141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3141" t="n">
+        <v>38231.67763972918</v>
+      </c>
+    </row>
+    <row r="3142">
+      <c r="A3142" s="1" t="n">
+        <v>3140</v>
+      </c>
+      <c r="B3142" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3142" t="n">
+        <v>38233.4</v>
+      </c>
+      <c r="D3142" t="n">
+        <v>38235.85</v>
+      </c>
+      <c r="E3142" t="n">
+        <v>38161.3</v>
+      </c>
+      <c r="F3142" t="n">
+        <v>38198.4</v>
+      </c>
+      <c r="G3142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3142" t="n">
+        <v>38220.58509315279</v>
+      </c>
+    </row>
+    <row r="3143">
+      <c r="A3143" s="1" t="n">
+        <v>3141</v>
+      </c>
+      <c r="B3143" s="2" t="n">
+        <v>44578</v>
+      </c>
+      <c r="C3143" t="n">
+        <v>38196.45</v>
+      </c>
+      <c r="D3143" t="n">
+        <v>38225.6</v>
+      </c>
+      <c r="E3143" t="n">
+        <v>38191.65</v>
+      </c>
+      <c r="F3143" t="n">
+        <v>38207.75</v>
+      </c>
+      <c r="G3143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3143" t="n">
+        <v>38216.30672876853</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>